<commit_message>
Adjust ELINK / "PCIEClockConfig" 	Name  = "{ CLOCK_SRC0, PCI_FUNCTION_NUMBER_PCH_PCIE_ROOT_PORT_1, 0 }," 	Name  = "{ CLOCK_SRC1, PCI_FUNCTION_NUMBER_PCH_PCIE_ROOT_PORT_2, 0 }," 	Name  = "{ CLOCK_SRC2, PCI_FUNCTION_NUMBER_PCH_PCIE_ROOT_PORT_3, 0 },"
</commit_message>
<xml_diff>
--- a/ReleaseHistory.xlsx
+++ b/ReleaseHistory.xlsx
@@ -174,12 +174,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">EE Reported :
 </t>
     </r>
@@ -210,7 +204,46 @@
         <family val="3"/>
         <charset val="136"/>
       </rPr>
-      <t>，时间很久</t>
+      <t xml:space="preserve">，时间很久
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Release [SZPRJM02]
+EE Reported : sata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">接口没有问题了，是设备的问题
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">EE Reported : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>网口只能抓到一个</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,6 +283,17 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="細明體"/>
       <family val="3"/>
       <charset val="136"/>
@@ -579,7 +623,7 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B12" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -633,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43273</v>
       </c>

</xml_diff>